<commit_message>
Added meeting action items
</commit_message>
<xml_diff>
--- a/Action Items/open_action_items.xlsx
+++ b/Action Items/open_action_items.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="9480" yWindow="0" windowWidth="25600" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="46">
   <si>
     <t>Item</t>
   </si>
@@ -136,6 +136,27 @@
   </si>
   <si>
     <t xml:space="preserve">BYU papers, UKFs, etc. </t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Trade Study on Hardware</t>
+  </si>
+  <si>
+    <t>Wait for customer verification of requirements before doing this</t>
+  </si>
+  <si>
+    <t>closed</t>
+  </si>
+  <si>
+    <t>Matt, Tyler, Taylor</t>
+  </si>
+  <si>
+    <t>Get quadrotor flying and pull data</t>
+  </si>
+  <si>
+    <t>Use vicon tutorial from Steve to pull data while quad is flying, import into matlab</t>
   </si>
 </sst>
 </file>
@@ -198,7 +219,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -216,6 +237,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -547,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -635,7 +657,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="C4" s="3">
         <v>42255</v>
@@ -874,6 +896,61 @@
       <c r="G14" s="5" t="s">
         <v>38</v>
       </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="5">
+        <v>14</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="6">
+        <v>42249</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="7">
+        <v>15</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="6">
+        <v>42262</v>
+      </c>
+      <c r="D16" s="6">
+        <v>42249</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Updated requirements and action items
</commit_message>
<xml_diff>
--- a/Action Items/open_action_items.xlsx
+++ b/Action Items/open_action_items.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="9480" yWindow="0" windowWidth="25600" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="47">
   <si>
     <t>Item</t>
   </si>
@@ -66,9 +66,6 @@
     <t>Have VM installed</t>
   </si>
   <si>
-    <t>Lit. Rev.: Visual Tracking/Odometery/Lens</t>
-  </si>
-  <si>
     <t>Austin</t>
   </si>
   <si>
@@ -93,9 +90,6 @@
     <t>Taylor</t>
   </si>
   <si>
-    <t>Lit. Rev.: Swarm Flight/Vis. Od.</t>
-  </si>
-  <si>
     <t>Prashant</t>
   </si>
   <si>
@@ -157,6 +151,15 @@
   </si>
   <si>
     <t>Use vicon tutorial from Steve to pull data while quad is flying, import into matlab</t>
+  </si>
+  <si>
+    <t>Lit. Rev: SLAM</t>
+  </si>
+  <si>
+    <t>Lit. Rev.: SLAM</t>
+  </si>
+  <si>
+    <t>Lit. Rev.: Visual Odemetry / SLAM</t>
   </si>
 </sst>
 </file>
@@ -572,7 +575,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -603,7 +606,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -626,7 +629,7 @@
         <v>8</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30">
@@ -649,7 +652,7 @@
         <v>10</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -657,7 +660,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C4" s="3">
         <v>42255</v>
@@ -672,7 +675,7 @@
         <v>13</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -713,10 +716,10 @@
         <v>12</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -733,13 +736,13 @@
         <v>42248</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="G7" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30">
@@ -756,13 +759,13 @@
         <v>42248</v>
       </c>
       <c r="E8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="G8" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="30">
@@ -779,13 +782,13 @@
         <v>42248</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -802,10 +805,10 @@
         <v>42248</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="G10" s="4"/>
     </row>
@@ -823,10 +826,10 @@
         <v>42248</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="G11" s="4"/>
     </row>
@@ -844,10 +847,10 @@
         <v>42248</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G12" s="4"/>
     </row>
@@ -865,13 +868,13 @@
         <v>42248</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -888,13 +891,13 @@
         <v>42248</v>
       </c>
       <c r="E14" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G14" s="5" t="s">
         <v>36</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -905,19 +908,19 @@
         <v>6</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D15" s="6">
         <v>42249</v>
       </c>
       <c r="E15" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G15" s="5" t="s">
         <v>39</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -934,13 +937,13 @@
         <v>42249</v>
       </c>
       <c r="E16" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G16" s="7" t="s">
         <v>43</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:7">

</xml_diff>

<commit_message>
Added quadrotor ukf model skeleton and updated open action items
</commit_message>
<xml_diff>
--- a/Action Items/open_action_items.xlsx
+++ b/Action Items/open_action_items.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="54">
   <si>
     <t>Item</t>
   </si>
@@ -132,12 +132,6 @@
     <t xml:space="preserve">BYU papers, UKFs, etc. </t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t>Trade Study on Hardware</t>
-  </si>
-  <si>
     <t>Wait for customer verification of requirements before doing this</t>
   </si>
   <si>
@@ -160,6 +154,33 @@
   </si>
   <si>
     <t>Lit. Rev.: Visual Odemetry / SLAM</t>
+  </si>
+  <si>
+    <t>review</t>
+  </si>
+  <si>
+    <t>Controls Team</t>
+  </si>
+  <si>
+    <t>Develop controller models</t>
+  </si>
+  <si>
+    <t>Presentation will be made to Dr. Frew on 9-15</t>
+  </si>
+  <si>
+    <t>SLAM Team</t>
+  </si>
+  <si>
+    <t>Trade Study on Hardware (onboard comps)</t>
+  </si>
+  <si>
+    <t>Prototype SLAM Algorithm on Laptop</t>
+  </si>
+  <si>
+    <t>Presentation will be made to Dr. Frew on 9-23</t>
+  </si>
+  <si>
+    <t>Order and receive onboard computers and sensors</t>
   </si>
 </sst>
 </file>
@@ -572,10 +593,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -614,7 +635,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="C2" s="3">
         <v>42251</v>
@@ -637,7 +658,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="C3" s="3">
         <v>42268</v>
@@ -660,7 +681,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C4" s="3">
         <v>42255</v>
@@ -683,7 +704,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="C5" s="3">
         <v>42255</v>
@@ -716,7 +737,7 @@
         <v>12</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>29</v>
@@ -785,7 +806,7 @@
         <v>19</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>31</v>
@@ -808,7 +829,7 @@
         <v>20</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G10" s="4"/>
     </row>
@@ -829,7 +850,7 @@
         <v>22</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G11" s="4"/>
     </row>
@@ -907,20 +928,20 @@
       <c r="B15" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>37</v>
+      <c r="C15" s="6">
+        <v>42258</v>
       </c>
       <c r="D15" s="6">
         <v>42249</v>
       </c>
       <c r="E15" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G15" s="5" t="s">
         <v>37</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -937,23 +958,81 @@
         <v>42249</v>
       </c>
       <c r="E16" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G16" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="F16" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
+      <c r="A17" s="7">
+        <v>16</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="6">
+        <v>42263</v>
+      </c>
+      <c r="D17" s="6">
+        <v>42255</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="5">
+        <v>17</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="6">
+        <v>42270</v>
+      </c>
+      <c r="D18" s="6">
+        <v>42255</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="30">
+      <c r="A19" s="5">
+        <v>18</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="6">
+        <v>42278</v>
+      </c>
+      <c r="D19" s="6">
+        <v>42255</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G19" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Updated action items, requirements list is in progress, minutes and hardware purchase list added
</commit_message>
<xml_diff>
--- a/Action Items/open_action_items.xlsx
+++ b/Action Items/open_action_items.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="62">
   <si>
     <t>Item</t>
   </si>
@@ -42,30 +42,15 @@
     <t>open</t>
   </si>
   <si>
-    <t>Austin/Drew</t>
-  </si>
-  <si>
-    <t>Meet with sponsors</t>
-  </si>
-  <si>
     <t>All</t>
   </si>
   <si>
-    <t>Scope document</t>
-  </si>
-  <si>
     <t xml:space="preserve">open </t>
   </si>
   <si>
     <t>Steve</t>
   </si>
   <si>
-    <t>Make a vicon tutorial</t>
-  </si>
-  <si>
-    <t>Have VM installed</t>
-  </si>
-  <si>
     <t>Austin</t>
   </si>
   <si>
@@ -99,15 +84,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Attendance of other team members is optional</t>
-  </si>
-  <si>
-    <t>Will be based on current understanding of requirements from Joe Tanners slides until further clarification is obtained from UTRC</t>
-  </si>
-  <si>
-    <t>Should be accessible to all with no vicon/linux experience</t>
-  </si>
-  <si>
     <t>Cheap lens parametrization, strategies for mitigating bad effects of cheap cameras</t>
   </si>
   <si>
@@ -132,12 +108,6 @@
     <t xml:space="preserve">BYU papers, UKFs, etc. </t>
   </si>
   <si>
-    <t>Wait for customer verification of requirements before doing this</t>
-  </si>
-  <si>
-    <t>closed</t>
-  </si>
-  <si>
     <t>Matt, Tyler, Taylor</t>
   </si>
   <si>
@@ -153,9 +123,6 @@
     <t>Lit. Rev.: SLAM</t>
   </si>
   <si>
-    <t>Lit. Rev.: Visual Odemetry / SLAM</t>
-  </si>
-  <si>
     <t>review</t>
   </si>
   <si>
@@ -168,26 +135,83 @@
     <t>Presentation will be made to Dr. Frew on 9-15</t>
   </si>
   <si>
-    <t>SLAM Team</t>
-  </si>
-  <si>
-    <t>Trade Study on Hardware (onboard comps)</t>
-  </si>
-  <si>
     <t>Prototype SLAM Algorithm on Laptop</t>
   </si>
   <si>
     <t>Presentation will be made to Dr. Frew on 9-23</t>
   </si>
   <si>
-    <t>Order and receive onboard computers and sensors</t>
+    <t>Drew/Austin</t>
+  </si>
+  <si>
+    <t>Create requirements document</t>
+  </si>
+  <si>
+    <t>Should flow down from given customer description</t>
+  </si>
+  <si>
+    <t>Create integration team</t>
+  </si>
+  <si>
+    <t>Should consist of one member of each current subteam lead by the SE</t>
+  </si>
+  <si>
+    <t>Nav. Team</t>
+  </si>
+  <si>
+    <t>Perform trade study on camera sensor setup, onboard computers, and rangefinders</t>
+  </si>
+  <si>
+    <t>Controls Team (Prashant)</t>
+  </si>
+  <si>
+    <t>Perform trade study on autopilots</t>
+  </si>
+  <si>
+    <t>Accelerometer performance, gyro performance, and computing power</t>
+  </si>
+  <si>
+    <t>Perform trade studies on SLAM solutions</t>
+  </si>
+  <si>
+    <t>Follow up with Zohaib on questions listed in 9/9 minutes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference Steve's parts list and a bluetooth telecon tool </t>
+  </si>
+  <si>
+    <t>Review project charter</t>
+  </si>
+  <si>
+    <t>Send revisions and suggestions to Drew</t>
+  </si>
+  <si>
+    <t>Task Level</t>
+  </si>
+  <si>
+    <t>Lit. Rev.: Visual Odometry / SLAM</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Complete purchase orders on onboard PCs and sensors</t>
+  </si>
+  <si>
+    <t>Reference map errors, position estimate errors, and projected run rate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -200,6 +224,22 @@
       <color theme="1"/>
       <name val="Cambria"/>
       <scheme val="major"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -240,30 +280,53 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="9">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -593,21 +656,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="39" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="72.33203125" customWidth="1"/>
+    <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22" customWidth="1"/>
+    <col min="7" max="7" width="47.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="72.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -624,67 +688,76 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="C2" s="3">
-        <v>42251</v>
+        <v>42262</v>
       </c>
       <c r="D2" s="3">
         <v>42248</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="30">
+        <v>59</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="C3" s="3">
-        <v>42268</v>
+        <v>42262</v>
       </c>
       <c r="D3" s="3">
         <v>42248</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>59</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="30">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="C4" s="3">
-        <v>42255</v>
+        <v>42262</v>
       </c>
       <c r="D4" s="3">
         <v>42248</v>
@@ -693,39 +766,47 @@
         <v>12</v>
       </c>
       <c r="F4" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="H4" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="30">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="C5" s="3">
-        <v>42255</v>
+        <v>42262</v>
       </c>
       <c r="D5" s="3">
         <v>42248</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="1:7">
+        <v>59</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C6" s="3">
         <v>42262</v>
@@ -734,16 +815,17 @@
         <v>42248</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>59</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -757,16 +839,17 @@
         <v>42248</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="30">
+        <v>59</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -780,16 +863,17 @@
         <v>42248</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="30">
+        <v>59</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" ht="30">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -806,233 +890,332 @@
         <v>19</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>59</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="3">
+      <c r="B10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="5">
         <v>42262</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="5">
         <v>42248</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G10" s="4"/>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="E10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="3">
+      <c r="B11" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="5">
         <v>42262</v>
       </c>
-      <c r="D11" s="3">
-        <v>42248</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="D11" s="5">
+        <v>42249</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="3">
-        <v>42262</v>
-      </c>
-      <c r="D12" s="3">
-        <v>42248</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G12" s="4"/>
-    </row>
-    <row r="13" spans="1:7" ht="30">
+      <c r="B12" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="5">
+        <v>42263</v>
+      </c>
+      <c r="D12" s="5">
+        <v>42255</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="3">
-        <v>42262</v>
-      </c>
-      <c r="D13" s="3">
-        <v>42248</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>32</v>
+      <c r="B13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="5">
+        <v>42270</v>
+      </c>
+      <c r="D13" s="5">
+        <v>42255</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="5">
+        <v>38</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="2">
         <v>13</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="6">
-        <v>42262</v>
-      </c>
-      <c r="D14" s="6">
-        <v>42248</v>
-      </c>
-      <c r="E14" s="5" t="s">
+      <c r="B14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="5">
+        <v>42263</v>
+      </c>
+      <c r="D14" s="5">
+        <v>42256</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="5">
+        <v>42263</v>
+      </c>
+      <c r="D15" s="5">
+        <v>42256</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="30">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="5">
+        <v>42263</v>
+      </c>
+      <c r="D16" s="5">
+        <v>42256</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H16" s="6"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="5">
+        <v>42263</v>
+      </c>
+      <c r="D17" s="5">
+        <v>42256</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="5">
+        <v>42263</v>
+      </c>
+      <c r="D18" s="5">
+        <v>42256</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="5">
+        <v>42263</v>
+      </c>
+      <c r="D19" s="5">
+        <v>42256</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H19" s="6"/>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="2">
+        <v>19</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="5">
+        <v>42263</v>
+      </c>
+      <c r="D20" s="5">
+        <v>42256</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="2">
+        <v>20</v>
+      </c>
+      <c r="B21" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F14" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="5">
-        <v>14</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="6">
-        <v>42258</v>
-      </c>
-      <c r="D15" s="6">
-        <v>42249</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="7">
-        <v>15</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="6">
-        <v>42262</v>
-      </c>
-      <c r="D16" s="6">
-        <v>42249</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="7">
-        <v>16</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="6">
+      <c r="C21" s="5">
         <v>42263</v>
       </c>
-      <c r="D17" s="6">
-        <v>42255</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="5">
-        <v>17</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="6">
-        <v>42270</v>
-      </c>
-      <c r="D18" s="6">
-        <v>42255</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="30">
-      <c r="A19" s="5">
-        <v>18</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="6">
-        <v>42278</v>
-      </c>
-      <c r="D19" s="6">
-        <v>42255</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F19" s="5" t="s">
+      <c r="D21" s="5">
+        <v>42256</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G21" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="G19" s="7"/>
+      <c r="H21" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added controls team action items
</commit_message>
<xml_diff>
--- a/Action Items/open_action_items.xlsx
+++ b/Action Items/open_action_items.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bryce\Documents\Flynet\Action Items\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="760" yWindow="740" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="765" yWindow="735" windowWidth="25605" windowHeight="16065" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="52">
   <si>
     <t>Item</t>
   </si>
@@ -145,6 +150,36 @@
   </si>
   <si>
     <t>Get turtlebots running</t>
+  </si>
+  <si>
+    <t>Bryce</t>
+  </si>
+  <si>
+    <t>SIL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIL </t>
+  </si>
+  <si>
+    <t xml:space="preserve">open </t>
+  </si>
+  <si>
+    <t>Prashant</t>
+  </si>
+  <si>
+    <t>Understand code currently onboard Pixhawk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matt  </t>
+  </si>
+  <si>
+    <t>Set up ROS and communication on Odroid</t>
+  </si>
+  <si>
+    <t>HIIGH</t>
+  </si>
+  <si>
+    <t>Develop control block diagram</t>
   </si>
 </sst>
 </file>
@@ -163,6 +198,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Cambria"/>
+      <family val="1"/>
       <scheme val="major"/>
     </font>
     <font>
@@ -309,6 +345,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -636,20 +680,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22" customWidth="1"/>
-    <col min="7" max="7" width="47.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="72.33203125" customWidth="1"/>
+    <col min="7" max="7" width="47.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="72.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -675,7 +719,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -701,7 +745,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="30">
+    <row r="3" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>3</v>
       </c>
@@ -727,7 +771,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>4</v>
       </c>
@@ -753,7 +797,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>7</v>
       </c>
@@ -779,7 +823,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>9</v>
       </c>
@@ -803,7 +847,7 @@
       </c>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>10</v>
       </c>
@@ -829,7 +873,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>11</v>
       </c>
@@ -855,7 +899,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>12</v>
       </c>
@@ -879,7 +923,7 @@
       </c>
       <c r="H9" s="11"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>13</v>
       </c>
@@ -903,7 +947,7 @@
       </c>
       <c r="H10" s="11"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>14</v>
       </c>
@@ -927,7 +971,7 @@
       </c>
       <c r="H11" s="11"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>15</v>
       </c>
@@ -951,7 +995,7 @@
       </c>
       <c r="H12" s="11"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>16</v>
       </c>
@@ -975,7 +1019,7 @@
       </c>
       <c r="H13" s="11"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>17</v>
       </c>
@@ -999,53 +1043,105 @@
       </c>
       <c r="H14" s="11"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>18</v>
       </c>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="B15" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="10">
+        <v>42270</v>
+      </c>
+      <c r="D15" s="10">
+        <v>42263</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>19</v>
       </c>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
+      <c r="B16" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="10">
+        <v>42270</v>
+      </c>
+      <c r="D16" s="10">
+        <v>42263</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>47</v>
+      </c>
       <c r="H16" s="11"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>20</v>
       </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
+      <c r="B17" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="10">
+        <v>42270</v>
+      </c>
+      <c r="D17" s="10">
+        <v>42263</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>49</v>
+      </c>
       <c r="H17" s="11"/>
     </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="6"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
+        <v>21</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="4">
+        <v>42270</v>
+      </c>
+      <c r="D18" s="4">
+        <v>42263</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>51</v>
+      </c>
       <c r="H18" s="5"/>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B19" s="11"/>
       <c r="C19" s="11"/>
       <c r="D19" s="11"/>
@@ -1054,7 +1150,7 @@
       <c r="G19" s="11"/>
       <c r="H19" s="11"/>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B20" s="11"/>
       <c r="C20" s="11"/>
       <c r="D20" s="11"/>
@@ -1063,7 +1159,7 @@
       <c r="G20" s="11"/>
       <c r="H20" s="11"/>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B21" s="11"/>
       <c r="C21" s="11"/>
       <c r="D21" s="11"/>
@@ -1072,7 +1168,7 @@
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B22" s="11"/>
       <c r="C22" s="11"/>
       <c r="D22" s="11"/>
@@ -1081,7 +1177,7 @@
       <c r="G22" s="11"/>
       <c r="H22" s="11"/>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B23" s="11"/>
       <c r="C23" s="11"/>
       <c r="D23" s="11"/>
@@ -1090,7 +1186,7 @@
       <c r="G23" s="11"/>
       <c r="H23" s="11"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B24" s="11"/>
       <c r="C24" s="11"/>
       <c r="D24" s="11"/>
@@ -1099,43 +1195,43 @@
       <c r="G24" s="11"/>
       <c r="H24" s="11"/>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
     </row>
-    <row r="33" spans="3:4">
+    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
     </row>
-    <row r="34" spans="3:4">
+    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C34" s="8"/>
     </row>
   </sheetData>

</xml_diff>